<commit_message>
Working on usage import.
</commit_message>
<xml_diff>
--- a/TestData/Eq Usage Post - Test.xlsx
+++ b/TestData/Eq Usage Post - Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GCIEQ\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\GCIEQ\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3295AD6-BD33-4C91-8C39-2698219231C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA62AA8C-7755-4298-A5E9-3890EBF1F112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1110" windowWidth="28020" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22185" yWindow="6780" windowWidth="22530" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eq Usage Post - 2024" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>sort_order_no</t>
   </si>
@@ -181,27 +181,9 @@
     <t>equip_end_time_military</t>
   </si>
   <si>
-    <t>1233</t>
-  </si>
-  <si>
-    <t>Batch No: 1233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P55       </t>
-  </si>
-  <si>
-    <t>2016 Dodge RAM 2500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       901</t>
-  </si>
-  <si>
     <t xml:space="preserve">         1</t>
   </si>
   <si>
-    <t xml:space="preserve">901-HOL   </t>
-  </si>
-  <si>
     <t xml:space="preserve">    4</t>
   </si>
   <si>
@@ -211,31 +193,64 @@
     <t>PAM</t>
   </si>
   <si>
-    <t>Total for Batch 1233:</t>
-  </si>
-  <si>
     <t xml:space="preserve">EQ </t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t xml:space="preserve">P88       </t>
-  </si>
-  <si>
-    <t>2022 Dodge Ram 2500 FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR3       </t>
-  </si>
-  <si>
-    <t>2007 Peterbilt Tractor (red)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    211530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1501.01   </t>
+    <t>1344</t>
+  </si>
+  <si>
+    <t>Batch No: 1344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    231648</t>
+  </si>
+  <si>
+    <t>Total for Batch 1344:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6521.03   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E39       </t>
+  </si>
+  <si>
+    <t>2021 Komatsu Hydraul Excavator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P91       </t>
+  </si>
+  <si>
+    <t>2022 RAM 2500 4x4 CrewC 8ftBd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    231659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3030.05   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P101      </t>
+  </si>
+  <si>
+    <t>2024 RAM 2500 - 7638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    231664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P76       </t>
+  </si>
+  <si>
+    <t>2020 RAM 2500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    231675</t>
   </si>
 </sst>
 </file>
@@ -272,9 +287,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA7"/>
+  <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -625,9 +641,9 @@
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1"/>
     <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="25" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="24" bestFit="1" customWidth="1"/>
@@ -697,7 +713,7 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
@@ -826,70 +842,82 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1344</v>
+      </c>
+      <c r="F2">
+        <v>346</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45611</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1233</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="N2">
+        <v>5201</v>
+      </c>
+      <c r="O2">
+        <v>5201</v>
+      </c>
+      <c r="P2">
+        <v>6036</v>
+      </c>
+      <c r="Q2">
+        <v>6036</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
+      <c r="T2">
+        <v>65</v>
+      </c>
+      <c r="U2">
+        <v>195</v>
+      </c>
+      <c r="V2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="1">
-        <v>45292</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2">
-        <v>10</v>
-      </c>
-      <c r="S2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2">
-        <v>5</v>
-      </c>
-      <c r="U2">
-        <v>50</v>
-      </c>
-      <c r="V2" t="s">
-        <v>62</v>
-      </c>
       <c r="AG2">
-        <v>13656.5</v>
+        <v>25856.55</v>
       </c>
       <c r="AJ2">
         <v>1582913.2</v>
       </c>
       <c r="AK2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="AM2">
         <v>0</v>
@@ -904,36 +932,36 @@
         <v>1</v>
       </c>
       <c r="AS2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="AT2">
         <v>0</v>
       </c>
       <c r="AW2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AZ2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1233</v>
+        <v>1344</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>347</v>
       </c>
       <c r="G3" t="s">
         <v>66</v>
@@ -942,46 +970,58 @@
         <v>67</v>
       </c>
       <c r="I3" s="1">
-        <v>45292</v>
+        <v>45611</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="M3" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="N3">
+        <v>5200</v>
+      </c>
+      <c r="O3">
+        <v>5200</v>
+      </c>
+      <c r="P3">
+        <v>6036</v>
+      </c>
+      <c r="Q3">
+        <v>6036</v>
       </c>
       <c r="R3">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="S3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="T3">
         <v>5</v>
       </c>
       <c r="U3">
-        <v>50</v>
+        <v>32.5</v>
       </c>
       <c r="V3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AG3">
-        <v>13656.5</v>
+        <v>25856.55</v>
       </c>
       <c r="AJ3">
         <v>1582913.2</v>
       </c>
       <c r="AK3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="AM3">
         <v>0</v>
@@ -1002,78 +1042,90 @@
         <v>0</v>
       </c>
       <c r="AW3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AZ3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1344</v>
+      </c>
+      <c r="F4">
+        <v>348</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="1">
+        <v>45611</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="L4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
         <v>54</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1233</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="1">
-        <v>45293</v>
-      </c>
-      <c r="J4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" t="s">
-        <v>60</v>
+      <c r="N4">
+        <v>5200</v>
+      </c>
+      <c r="O4">
+        <v>5200</v>
+      </c>
+      <c r="P4">
+        <v>6036</v>
+      </c>
+      <c r="Q4">
+        <v>6036</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="S4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="T4">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="U4">
-        <v>70</v>
+        <v>7.5</v>
       </c>
       <c r="V4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AG4">
-        <v>13656.5</v>
+        <v>25856.55</v>
       </c>
       <c r="AJ4">
         <v>1582913.2</v>
       </c>
       <c r="AK4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="AM4">
         <v>0</v>
@@ -1088,84 +1140,96 @@
         <v>1</v>
       </c>
       <c r="AS4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AT4">
         <v>0</v>
       </c>
       <c r="AW4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AZ4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1344</v>
+      </c>
+      <c r="F5">
+        <v>349</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45611</v>
+      </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="L5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
         <v>54</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1233</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="N5">
+        <v>5200</v>
+      </c>
+      <c r="O5">
+        <v>5200</v>
+      </c>
+      <c r="P5">
+        <v>6036</v>
+      </c>
+      <c r="Q5">
+        <v>6036</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
         <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="1">
-        <v>45658</v>
-      </c>
-      <c r="J5" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5" t="s">
-        <v>61</v>
       </c>
       <c r="T5">
         <v>5</v>
       </c>
       <c r="U5">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="V5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AG5">
-        <v>13656.5</v>
+        <v>25856.55</v>
       </c>
       <c r="AJ5">
         <v>1582913.2</v>
       </c>
       <c r="AK5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="AM5">
         <v>0</v>
@@ -1180,84 +1244,96 @@
         <v>1</v>
       </c>
       <c r="AS5" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="AT5">
         <v>0</v>
       </c>
       <c r="AW5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AZ5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1344</v>
+      </c>
+      <c r="F6">
+        <v>350</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45613</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="L6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" t="s">
         <v>54</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1233</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="1">
-        <v>45658</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" t="s">
-        <v>60</v>
+      <c r="N6">
+        <v>5201</v>
+      </c>
+      <c r="O6">
+        <v>5201</v>
+      </c>
+      <c r="P6">
+        <v>6036</v>
+      </c>
+      <c r="Q6">
+        <v>6036</v>
       </c>
       <c r="R6">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="S6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="T6">
         <v>5</v>
       </c>
       <c r="U6">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="V6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AG6">
-        <v>13656.5</v>
+        <v>25856.55</v>
       </c>
       <c r="AJ6">
         <v>1582913.2</v>
       </c>
       <c r="AK6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -1272,108 +1348,16 @@
         <v>1</v>
       </c>
       <c r="AS6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AT6">
         <v>0</v>
       </c>
       <c r="AW6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AZ6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1350</v>
-      </c>
-      <c r="B7">
-        <v>1350</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1233</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="1">
-        <v>45658</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" t="s">
         <v>58</v>
-      </c>
-      <c r="L7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" t="s">
-        <v>60</v>
-      </c>
-      <c r="R7">
-        <v>2</v>
-      </c>
-      <c r="S7" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7">
-        <v>35</v>
-      </c>
-      <c r="U7">
-        <v>70</v>
-      </c>
-      <c r="V7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG7">
-        <v>13656.5</v>
-      </c>
-      <c r="AJ7">
-        <v>1582913.2</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AN7">
-        <v>0</v>
-      </c>
-      <c r="AO7">
-        <v>1</v>
-      </c>
-      <c r="AR7">
-        <v>1</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Jupyter for eq usage import
</commit_message>
<xml_diff>
--- a/TestData/Eq Usage Post - Test.xlsx
+++ b/TestData/Eq Usage Post - Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\GCIEQ\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA62AA8C-7755-4298-A5E9-3890EBF1F112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF4C11D-1C9B-4BE8-BA7C-1FC5E8283BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22185" yWindow="6780" windowWidth="22530" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23940" yWindow="4170" windowWidth="22530" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eq Usage Post - 2024" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>sort_order_no</t>
   </si>
@@ -625,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA6"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1360,6 +1360,110 @@
         <v>58</v>
       </c>
     </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1345</v>
+      </c>
+      <c r="B7">
+        <v>1345</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1345</v>
+      </c>
+      <c r="F7">
+        <v>350</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="1">
+        <v>45613</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7">
+        <v>5201</v>
+      </c>
+      <c r="O7">
+        <v>5201</v>
+      </c>
+      <c r="P7">
+        <v>6036</v>
+      </c>
+      <c r="Q7">
+        <v>6036</v>
+      </c>
+      <c r="R7">
+        <v>0.01</v>
+      </c>
+      <c r="S7" t="s">
+        <v>55</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>0.05</v>
+      </c>
+      <c r="V7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG7">
+        <v>25856.55</v>
+      </c>
+      <c r="AJ7">
+        <v>1582913.2</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>